<commit_message>
Upddated Excel and some plots
</commit_message>
<xml_diff>
--- a/Lab06-filter_simulation/Values.xlsx
+++ b/Lab06-filter_simulation/Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g_tec/Git/CircuitDesign/Lab06-filter_simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D51361-7D38-364F-B814-95D93AA9DE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA24548-6A72-7044-AAF9-8FC56C5DFFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="1040" windowWidth="32280" windowHeight="23840" xr2:uid="{127C26D3-BB75-3F47-9D83-6B7AE89B4662}"/>
+    <workbookView xWindow="160" yWindow="1040" windowWidth="40800" windowHeight="23840" activeTab="4" xr2:uid="{127C26D3-BB75-3F47-9D83-6B7AE89B4662}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="195">
   <si>
     <t>V(Net-_L1-Pad1_) (gain)</t>
   </si>
@@ -615,16 +615,110 @@
   <si>
     <t>Phase</t>
   </si>
+  <si>
+    <t>Degree symbol ° added later in LaTeX with fn key insert</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>Simulated</t>
+  </si>
+  <si>
+    <t>795,8Hz</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>fra teoretisk</t>
+  </si>
+  <si>
+    <t>Deviation</t>
+  </si>
+  <si>
+    <t>Generator</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>2,00V</t>
+  </si>
+  <si>
+    <t>1,41V</t>
+  </si>
+  <si>
+    <t>1,80V</t>
+  </si>
+  <si>
+    <t>1,94V</t>
+  </si>
+  <si>
+    <t>59,1mV</t>
+  </si>
+  <si>
+    <t>1,42V</t>
+  </si>
+  <si>
+    <t>584mV</t>
+  </si>
+  <si>
+    <t>1,99V</t>
+  </si>
+  <si>
+    <t>9,61mV</t>
+  </si>
+  <si>
+    <t>1,76V</t>
+  </si>
+  <si>
+    <t>4,81kHz</t>
+  </si>
+  <si>
+    <t>4,82kHz</t>
+  </si>
+  <si>
+    <t>4,84kHz</t>
+  </si>
+  <si>
+    <t>1,8V</t>
+  </si>
+  <si>
+    <t>58,4mV</t>
+  </si>
+  <si>
+    <t>1,07kHz</t>
+  </si>
+  <si>
+    <t>1,073kHz</t>
+  </si>
+  <si>
+    <t>-0,28%</t>
+  </si>
+  <si>
+    <t>1,83V</t>
+  </si>
+  <si>
+    <t>approx 0</t>
+  </si>
+  <si>
+    <t>u replaced by µ inside editor later</t>
+  </si>
+  <si>
+    <t>approx replaced by \approx in editor later</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -657,13 +751,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9795"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -694,7 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -706,6 +818,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,6 +847,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9795"/>
+      <color rgb="FFFF7E79"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1041,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCCEA5A-D1F4-4046-AE71-99F4DED31528}">
-  <dimension ref="B4:K61"/>
+  <dimension ref="B4:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="182" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:K7"/>
+    <sheetView topLeftCell="A11" zoomScale="171" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,7 +1196,7 @@
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -1068,7 +1208,7 @@
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1082,7 +1222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -1105,7 +1245,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -1124,11 +1264,14 @@
       <c r="J7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K7" s="8">
+        <v>44.956000000000003</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>1</v>
       </c>
@@ -1136,7 +1279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1166,7 +1309,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
@@ -1181,8 +1324,17 @@
       <c r="F13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I13" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>20</v>
       </c>
@@ -1192,20 +1344,33 @@
       <c r="F14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I14" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="11">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="4">
-        <f>E14/E13</f>
-        <v>1.001539737964426</v>
+        <f>(E14-E13)/E13</f>
+        <v>1.53973796442601E-3</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>1</v>
       </c>
@@ -1213,7 +1378,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
@@ -1229,7 +1394,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
@@ -1245,7 +1410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>29</v>
       </c>
@@ -1261,7 +1426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
@@ -1277,7 +1442,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>33</v>
       </c>
@@ -1293,7 +1458,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
@@ -1309,7 +1474,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -1322,8 +1487,17 @@
       <c r="E26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I26" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>1</v>
       </c>
@@ -1336,8 +1510,17 @@
       <c r="E27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I27" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>2</v>
       </c>
@@ -1351,7 +1534,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>43</v>
       </c>
@@ -1365,7 +1548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>1</v>
       </c>
@@ -1373,7 +1556,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>50</v>
       </c>
@@ -1389,7 +1572,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>25</v>
       </c>
@@ -1405,7 +1588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>29</v>
       </c>
@@ -1421,7 +1604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>32</v>
       </c>
@@ -1437,7 +1620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>33</v>
       </c>
@@ -1453,7 +1636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>35</v>
       </c>
@@ -1469,7 +1652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>5</v>
       </c>
@@ -1482,8 +1665,17 @@
       <c r="E40" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I40" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>1</v>
       </c>
@@ -1496,8 +1688,17 @@
       <c r="E41" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I41" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>2</v>
       </c>
@@ -1511,7 +1712,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>43</v>
       </c>
@@ -1525,7 +1726,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>1</v>
       </c>
@@ -1533,7 +1734,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>50</v>
       </c>
@@ -1549,7 +1750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
         <v>25</v>
       </c>
@@ -1565,7 +1766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>29</v>
       </c>
@@ -1581,7 +1782,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>32</v>
       </c>
@@ -1597,7 +1798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>33</v>
       </c>
@@ -1613,7 +1814,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>35</v>
       </c>
@@ -1629,7 +1830,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>5</v>
       </c>
@@ -1642,8 +1843,17 @@
       <c r="E54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I54" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>1</v>
       </c>
@@ -1656,8 +1866,17 @@
       <c r="E55" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I55" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>2</v>
       </c>
@@ -1671,7 +1890,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>43</v>
       </c>
@@ -1685,7 +1904,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>1</v>
       </c>
@@ -1693,9 +1912,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C61" s="7"/>
     </row>
@@ -1731,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B58625-EFAA-1249-BD03-9379597038EA}">
-  <dimension ref="B4:F61"/>
+  <dimension ref="B4:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="356" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1746,7 +1965,7 @@
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1754,7 +1973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1767,8 +1986,17 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -1781,8 +2009,20 @@
       <c r="E6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>-44.936</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -1796,7 +2036,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2</v>
       </c>
@@ -1804,7 +2044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1819,7 +2059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1833,8 +2073,17 @@
       <c r="F12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H12" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
@@ -1849,8 +2098,17 @@
       <c r="F13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H13" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="11">
+        <v>-2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>20</v>
       </c>
@@ -1861,19 +2119,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="4">
-        <f>E14/E13</f>
-        <v>0.99776982678011827</v>
+        <f>(E14-E13)/E13</f>
+        <v>-2.2301732198817415E-3</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>2</v>
       </c>
@@ -1881,7 +2139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
@@ -1897,7 +2155,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
@@ -1913,7 +2171,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>29</v>
       </c>
@@ -1929,7 +2187,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
@@ -1945,7 +2203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>33</v>
       </c>
@@ -1961,7 +2219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
@@ -1977,7 +2235,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -1990,8 +2248,17 @@
       <c r="E26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H26" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>1</v>
       </c>
@@ -2004,8 +2271,17 @@
       <c r="E27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H27" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>2</v>
       </c>
@@ -2019,7 +2295,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>43</v>
       </c>
@@ -2033,7 +2309,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>2</v>
       </c>
@@ -2041,7 +2317,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>50</v>
       </c>
@@ -2057,7 +2333,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>25</v>
       </c>
@@ -2073,7 +2349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>29</v>
       </c>
@@ -2089,7 +2365,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>32</v>
       </c>
@@ -2105,7 +2381,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>33</v>
       </c>
@@ -2121,7 +2397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>35</v>
       </c>
@@ -2137,7 +2413,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>5</v>
       </c>
@@ -2150,8 +2426,17 @@
       <c r="E40" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H40" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>1</v>
       </c>
@@ -2164,8 +2449,17 @@
       <c r="E41" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H41" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>2</v>
       </c>
@@ -2179,7 +2473,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>43</v>
       </c>
@@ -2193,7 +2487,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>2</v>
       </c>
@@ -2201,7 +2495,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>50</v>
       </c>
@@ -2217,7 +2511,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
         <v>25</v>
       </c>
@@ -2233,7 +2527,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>29</v>
       </c>
@@ -2249,7 +2543,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>32</v>
       </c>
@@ -2265,7 +2559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>33</v>
       </c>
@@ -2281,7 +2575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>35</v>
       </c>
@@ -2297,7 +2591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>5</v>
       </c>
@@ -2310,8 +2604,17 @@
       <c r="E54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H54" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>1</v>
       </c>
@@ -2324,8 +2627,17 @@
       <c r="E55" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H55" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>2</v>
       </c>
@@ -2339,7 +2651,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>43</v>
       </c>
@@ -2353,7 +2665,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>2</v>
       </c>
@@ -2361,9 +2673,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C61" s="7"/>
     </row>
@@ -2398,10 +2710,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCCB6D8-CEAA-1C4B-8107-5F49A2FA7454}">
-  <dimension ref="B4:F61"/>
+  <dimension ref="B4:L61"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2413,7 +2725,7 @@
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>3</v>
       </c>
@@ -2421,7 +2733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -2434,8 +2746,17 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -2448,8 +2769,20 @@
       <c r="E6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>-44.923000000000002</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -2463,7 +2796,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>3</v>
       </c>
@@ -2471,7 +2804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>85</v>
       </c>
@@ -2486,7 +2819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>86</v>
       </c>
@@ -2500,8 +2833,17 @@
       <c r="F12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H12" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>87</v>
       </c>
@@ -2516,8 +2858,17 @@
       <c r="F13" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H13" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="J13" s="11">
+        <v>-2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>20</v>
       </c>
@@ -2528,19 +2879,19 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="4">
-        <f>E14/E13</f>
-        <v>0.99733000380861558</v>
+        <f>(E14-E13)/E13</f>
+        <v>-2.669996191384427E-3</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>3</v>
       </c>
@@ -2548,7 +2899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
@@ -2564,7 +2915,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
@@ -2580,7 +2931,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>29</v>
       </c>
@@ -2596,7 +2947,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
@@ -2612,7 +2963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>33</v>
       </c>
@@ -2628,7 +2979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
@@ -2644,7 +2995,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -2657,8 +3008,17 @@
       <c r="E26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H26" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>1</v>
       </c>
@@ -2671,8 +3031,17 @@
       <c r="E27" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H27" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>2</v>
       </c>
@@ -2686,7 +3055,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>43</v>
       </c>
@@ -2700,7 +3069,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>3</v>
       </c>
@@ -2708,7 +3077,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>50</v>
       </c>
@@ -2724,7 +3093,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>25</v>
       </c>
@@ -2740,7 +3109,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>29</v>
       </c>
@@ -2756,7 +3125,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>32</v>
       </c>
@@ -2772,7 +3141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>33</v>
       </c>
@@ -2788,7 +3157,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>35</v>
       </c>
@@ -2804,7 +3173,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>5</v>
       </c>
@@ -2817,8 +3186,17 @@
       <c r="E40" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H40" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>1</v>
       </c>
@@ -2831,8 +3209,17 @@
       <c r="E41" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H41" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>2</v>
       </c>
@@ -2846,7 +3233,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>43</v>
       </c>
@@ -2860,7 +3247,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>3</v>
       </c>
@@ -2868,7 +3255,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>50</v>
       </c>
@@ -2884,7 +3271,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
         <v>25</v>
       </c>
@@ -2900,7 +3287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>29</v>
       </c>
@@ -2916,7 +3303,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>32</v>
       </c>
@@ -2932,7 +3319,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>33</v>
       </c>
@@ -2948,7 +3335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>35</v>
       </c>
@@ -2964,7 +3351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>5</v>
       </c>
@@ -2977,8 +3364,17 @@
       <c r="E54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H54" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>1</v>
       </c>
@@ -2991,8 +3387,17 @@
       <c r="E55" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H55" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>2</v>
       </c>
@@ -3006,7 +3411,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>43</v>
       </c>
@@ -3020,7 +3425,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>3</v>
       </c>
@@ -3028,7 +3433,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
         <v>79</v>
       </c>
@@ -3065,10 +3470,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8120D559-63A7-AA4E-8ED5-BB00FDB27C57}">
-  <dimension ref="B4:F61"/>
+  <dimension ref="B4:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView zoomScale="159" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3080,7 +3485,7 @@
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>4</v>
       </c>
@@ -3088,7 +3493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -3101,8 +3506,17 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -3115,8 +3529,20 @@
       <c r="E6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>44.898000000000003</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -3130,7 +3556,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>4</v>
       </c>
@@ -3138,7 +3564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>85</v>
       </c>
@@ -3153,7 +3579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>86</v>
       </c>
@@ -3167,8 +3593,17 @@
       <c r="F12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H12" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>87</v>
       </c>
@@ -3183,8 +3618,17 @@
       <c r="F13" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H13" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" s="11">
+        <v>3.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>20</v>
       </c>
@@ -3195,19 +3639,19 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="4">
-        <f>E14/E13</f>
-        <v>1.0035503572627233</v>
+        <f>(E14-E13)/E13</f>
+        <v>3.5503572627234143E-3</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>4</v>
       </c>
@@ -3215,7 +3659,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
@@ -3231,7 +3675,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
@@ -3247,7 +3691,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>29</v>
       </c>
@@ -3263,7 +3707,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
@@ -3279,7 +3723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>33</v>
       </c>
@@ -3295,7 +3739,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
@@ -3311,7 +3755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -3324,8 +3768,17 @@
       <c r="E26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H26" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>1</v>
       </c>
@@ -3338,8 +3791,17 @@
       <c r="E27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H27" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>2</v>
       </c>
@@ -3353,7 +3815,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>43</v>
       </c>
@@ -3367,7 +3829,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>4</v>
       </c>
@@ -3375,7 +3837,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>50</v>
       </c>
@@ -3391,7 +3853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>25</v>
       </c>
@@ -3407,7 +3869,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>29</v>
       </c>
@@ -3423,7 +3885,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>32</v>
       </c>
@@ -3439,7 +3901,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>33</v>
       </c>
@@ -3455,7 +3917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>35</v>
       </c>
@@ -3471,7 +3933,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>5</v>
       </c>
@@ -3484,8 +3946,17 @@
       <c r="E40" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H40" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>1</v>
       </c>
@@ -3498,8 +3969,17 @@
       <c r="E41" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H41" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>2</v>
       </c>
@@ -3513,7 +3993,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>43</v>
       </c>
@@ -3527,7 +4007,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>4</v>
       </c>
@@ -3535,7 +4015,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>50</v>
       </c>
@@ -3551,7 +4031,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
         <v>25</v>
       </c>
@@ -3567,7 +4047,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>29</v>
       </c>
@@ -3583,7 +4063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>32</v>
       </c>
@@ -3599,7 +4079,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>33</v>
       </c>
@@ -3615,7 +4095,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>35</v>
       </c>
@@ -3631,7 +4111,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>5</v>
       </c>
@@ -3644,8 +4124,17 @@
       <c r="E54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H54" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>1</v>
       </c>
@@ -3658,8 +4147,17 @@
       <c r="E55" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H55" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>2</v>
       </c>
@@ -3673,7 +4171,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>43</v>
       </c>
@@ -3687,7 +4185,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>4</v>
       </c>
@@ -3695,7 +4193,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
         <v>58</v>
       </c>
@@ -3734,8 +4232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF21DCC8-4380-9A47-85BC-FCBB6F89D2DA}">
   <dimension ref="B4:O61"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="142" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54:J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3888,6 +4386,18 @@
       <c r="C10" t="s">
         <v>142</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="11" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
@@ -3903,8 +4413,18 @@
       <c r="F11" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="H11" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
@@ -3920,8 +4440,6 @@
       <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
@@ -3938,8 +4456,6 @@
       <c r="F13" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
@@ -3952,17 +4468,35 @@
       <c r="F14" t="s">
         <v>19</v>
       </c>
+      <c r="H14" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="4">
-        <f>E14/E13</f>
-        <v>0.99718327650188454</v>
+        <f>(E14-E13)/E13</f>
+        <v>-2.8167234981154648E-3</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>190</v>
       </c>
       <c r="K15" s="4"/>
     </row>
@@ -3970,7 +4504,7 @@
       <c r="E16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>4</v>
       </c>
@@ -3979,7 +4513,7 @@
       </c>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
@@ -3995,7 +4529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
@@ -4012,7 +4546,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>29</v>
       </c>
@@ -4029,7 +4563,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
@@ -4046,7 +4580,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>33</v>
       </c>
@@ -4063,7 +4597,7 @@
       </c>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
@@ -4080,7 +4614,7 @@
       </c>
       <c r="K24" s="5"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -4093,8 +4627,17 @@
       <c r="E26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H26" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>1</v>
       </c>
@@ -4107,8 +4650,20 @@
       <c r="E27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H27" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="L27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>2</v>
       </c>
@@ -4122,7 +4677,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>43</v>
       </c>
@@ -4136,7 +4691,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>4</v>
       </c>
@@ -4259,6 +4814,15 @@
       <c r="E40" t="s">
         <v>48</v>
       </c>
+      <c r="H40" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41">
@@ -4273,6 +4837,15 @@
       <c r="E41" t="s">
         <v>42</v>
       </c>
+      <c r="H41" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B42">
@@ -4424,6 +4997,15 @@
       <c r="E54" t="s">
         <v>48</v>
       </c>
+      <c r="H54" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55">
@@ -4438,6 +5020,15 @@
       <c r="E55" t="s">
         <v>42</v>
       </c>
+      <c r="H55" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56">
@@ -4484,7 +5075,7 @@
       <c r="I61" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="23">
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
@@ -4496,9 +5087,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B52:C52"/>
@@ -4513,5 +5101,8 @@
     <mergeCell ref="B23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="J15" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>